<commit_message>
fesco letter tmp cells content minor fix
</commit_message>
<xml_diff>
--- a/templates/Fesco_Letter.xlsx
+++ b/templates/Fesco_Letter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A4ED5A-5FAC-4F67-82C3-B81B523074B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AABF9D4-2D61-4E3B-863D-9A90321147A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Fesco_Letter" sheetId="1" r:id="rId1"/>
@@ -121,13 +121,13 @@
     <t>ООО "Дальрефтранс"</t>
   </si>
   <si>
-    <t>Болотову А.С.</t>
-  </si>
-  <si>
     <t>Уважаемый Александр Сергеевич !</t>
   </si>
   <si>
     <t>№</t>
+  </si>
+  <si>
+    <t>Болотину А.С.</t>
   </si>
 </sst>
 </file>
@@ -297,29 +297,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -698,7 +698,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -751,38 +751,38 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="G11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="G12" s="20"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="25" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="G12" s="21"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:18" ht="53.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="A14" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:18" s="5" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
@@ -793,10 +793,10 @@
       <c r="D15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
@@ -823,10 +823,10 @@
       <c r="D16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="27"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="8" t="s">
         <v>13</v>
       </c>
@@ -861,15 +861,15 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" s="17" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
+      <c r="A20" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
@@ -886,15 +886,15 @@
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
+      <c r="A23" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
@@ -946,19 +946,19 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="A31" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:13" ht="4.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
@@ -1046,7 +1046,7 @@
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="E15:F15"/>
   </mergeCells>
-  <conditionalFormatting sqref="A17:G18 G16 A16:E16">
+  <conditionalFormatting sqref="A16:E16 G16 A17:G18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
export fca contract tmp updated
</commit_message>
<xml_diff>
--- a/templates/Fesco_Letter.xlsx
+++ b/templates/Fesco_Letter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AABF9D4-2D61-4E3B-863D-9A90321147A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0322EDD9-687C-4E3F-BBDE-8ADD44A7F06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Fesco_Letter" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="Грузовые_борт_склад">Fesco_Letter!$A$25</definedName>
     <definedName name="Грузовые_склад_авто">Fesco_Letter!$A$26</definedName>
     <definedName name="Имя_представитель">Fesco_Letter!#REF!</definedName>
-    <definedName name="Исполнитель_информация">Fesco_Letter!$A$28</definedName>
+    <definedName name="Исполнитель_информация">Fesco_Letter!#REF!</definedName>
     <definedName name="Контрольный_звонок">Fesco_Letter!#REF!</definedName>
     <definedName name="Номер_письма">Fesco_Letter!$A$9</definedName>
     <definedName name="Образцы_выдача">Fesco_Letter!$A$19</definedName>
@@ -38,8 +38,8 @@
     <definedName name="Письмо_описание_подвал">Fesco_Letter!$A$21</definedName>
     <definedName name="Письмо_описание_шапка">Fesco_Letter!$A$14</definedName>
     <definedName name="Письмо_описание_шапка_приветствие">Fesco_Letter!$A$13</definedName>
-    <definedName name="Письмо_температура">Fesco_Letter!$A$31</definedName>
-    <definedName name="Письмо_электропитание">Fesco_Letter!$A$30</definedName>
+    <definedName name="Письмо_температура">Fesco_Letter!$A$28</definedName>
+    <definedName name="Письмо_электропитание">Fesco_Letter!$A$27</definedName>
     <definedName name="Подписант">Fesco_Letter!$G$34</definedName>
     <definedName name="Подписант_комментарий">Fesco_Letter!$A$34</definedName>
     <definedName name="Покупатель_телефон">Fesco_Letter!$A$24</definedName>
@@ -48,7 +48,7 @@
     <definedName name="Порт_почта">Fesco_Letter!$G$12</definedName>
     <definedName name="Расходы_компания">Fesco_Letter!$A$22</definedName>
     <definedName name="Телефон_представитель">Fesco_Letter!#REF!</definedName>
-    <definedName name="Хранение">Fesco_Letter!$A$27</definedName>
+    <definedName name="Хранение">Fesco_Letter!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Котов М.Н.</t>
   </si>
@@ -240,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -320,6 +320,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -698,7 +701,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -923,37 +926,35 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" s="17" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="17" t="s">
-        <v>6</v>
-      </c>
+    <row r="27" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" s="17" customFormat="1" ht="55.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="11"/>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E29" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="19.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="11"/>
-    </row>
+    <row r="30" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
@@ -1041,10 +1042,11 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A27:G27"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:E16 G16 A17:G18">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">

</xml_diff>

<commit_message>
fescco letter grouping fixed
</commit_message>
<xml_diff>
--- a/templates/Fesco_Letter.xlsx
+++ b/templates/Fesco_Letter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49374673-27AB-43AE-9321-8208B6F0D645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C15E0F-3007-4E89-BFD3-AFB038E8F40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16035" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="27076" windowHeight="16395" xr2:uid="{2E466B64-48C3-4933-967A-89DBEAC52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Fesco_Letter" sheetId="1" r:id="rId1"/>
@@ -18,35 +18,35 @@
   <definedNames>
     <definedName name="Banner_end">Fesco_Letter!$G$8</definedName>
     <definedName name="Banner_start">Fesco_Letter!$A$1</definedName>
-    <definedName name="Merge_end">Fesco_Letter!$A$33</definedName>
-    <definedName name="Pg_end">Fesco_Letter!$G$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Fesco_Letter!$A$1:$G$43</definedName>
-    <definedName name="Seal_seller_end">Fesco_Letter!$F$34</definedName>
-    <definedName name="Seal_seller_start">Fesco_Letter!$E$29</definedName>
-    <definedName name="Sign_seller_end">Fesco_Letter!$F$33</definedName>
-    <definedName name="Sign_seller_start">Fesco_Letter!$E$33</definedName>
-    <definedName name="Выгрузка_ответственный">Fesco_Letter!$A$23</definedName>
-    <definedName name="Грузовые_борт_склад">Fesco_Letter!$A$25</definedName>
-    <definedName name="Грузовые_склад_авто">Fesco_Letter!$A$26</definedName>
+    <definedName name="Merge_end">Fesco_Letter!$A$31</definedName>
+    <definedName name="Pg_end">Fesco_Letter!$G$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Fesco_Letter!$A$1:$G$41</definedName>
+    <definedName name="Seal_seller_end">Fesco_Letter!$F$32</definedName>
+    <definedName name="Seal_seller_start">Fesco_Letter!$E$27</definedName>
+    <definedName name="Sign_seller_end">Fesco_Letter!$F$31</definedName>
+    <definedName name="Sign_seller_start">Fesco_Letter!$E$31</definedName>
+    <definedName name="Выгрузка_ответственный">Fesco_Letter!$A$21</definedName>
+    <definedName name="Грузовые_борт_склад">Fesco_Letter!$A$23</definedName>
+    <definedName name="Грузовые_склад_авто">Fesco_Letter!$A$24</definedName>
     <definedName name="Имя_представитель">Fesco_Letter!#REF!</definedName>
     <definedName name="Исполнитель_информация">Fesco_Letter!#REF!</definedName>
     <definedName name="Контрольный_звонок">Fesco_Letter!#REF!</definedName>
     <definedName name="Номер_письма">Fesco_Letter!$A$9</definedName>
-    <definedName name="Образцы_выдача">Fesco_Letter!$A$19</definedName>
-    <definedName name="Образцы_подвал">Fesco_Letter!$A$20</definedName>
+    <definedName name="Образцы_выдача">Fesco_Letter!$A$17</definedName>
+    <definedName name="Образцы_подвал">Fesco_Letter!$A$18</definedName>
     <definedName name="Письмо_массив">Fesco_Letter!$A$16</definedName>
-    <definedName name="Письмо_описание_подвал">Fesco_Letter!$A$21</definedName>
+    <definedName name="Письмо_описание_подвал">Fesco_Letter!$A$19</definedName>
     <definedName name="Письмо_описание_шапка">Fesco_Letter!$A$14</definedName>
     <definedName name="Письмо_описание_шапка_приветствие">Fesco_Letter!$A$13</definedName>
-    <definedName name="Письмо_температура">Fesco_Letter!$A$28</definedName>
-    <definedName name="Письмо_электропитание">Fesco_Letter!$A$27</definedName>
-    <definedName name="Подписант">Fesco_Letter!$G$34</definedName>
-    <definedName name="Подписант_комментарий">Fesco_Letter!$A$34</definedName>
-    <definedName name="Покупатель_телефон">Fesco_Letter!$A$24</definedName>
+    <definedName name="Письмо_температура">Fesco_Letter!$A$26</definedName>
+    <definedName name="Письмо_электропитание">Fesco_Letter!$A$25</definedName>
+    <definedName name="Подписант">Fesco_Letter!$G$32</definedName>
+    <definedName name="Подписант_комментарий">Fesco_Letter!$A$32</definedName>
+    <definedName name="Покупатель_телефон">Fesco_Letter!$A$22</definedName>
     <definedName name="Порт">Fesco_Letter!$G$10</definedName>
     <definedName name="Порт_директор">Fesco_Letter!$G$11</definedName>
     <definedName name="Порт_почта">Fesco_Letter!$G$12</definedName>
-    <definedName name="Расходы_компания">Fesco_Letter!$A$22</definedName>
+    <definedName name="Расходы_компания">Fesco_Letter!$A$20</definedName>
     <definedName name="Телефон_представитель">Fesco_Letter!#REF!</definedName>
     <definedName name="Хранение">Fesco_Letter!#REF!</definedName>
   </definedNames>
@@ -240,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -256,9 +256,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -320,9 +317,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -698,10 +692,10 @@
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -727,10 +721,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="11"/>
+      <c r="A1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:18" ht="108.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
@@ -747,8 +741,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="F10" s="14"/>
-      <c r="G10" s="15" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -758,30 +752,30 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="G12" s="20"/>
+      <c r="G12" s="19"/>
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:18" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
     </row>
     <row r="14" spans="1:18" ht="53.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
+      <c r="A14" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:18" s="5" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
@@ -796,10 +790,10 @@
       <c r="D15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="27"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="4" t="s">
         <v>4</v>
       </c>
@@ -814,264 +808,245 @@
       <c r="R15"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="8" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="6"/>
+    <row r="17" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" s="16" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
     </row>
     <row r="19" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" s="17" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
+      <c r="A21" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
+      <c r="A23" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="26" spans="1:7" ht="0.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-    </row>
-    <row r="28" spans="1:7" s="17" customFormat="1" ht="55.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="11"/>
-      <c r="F28"/>
-      <c r="G28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="E29" s="11" t="s">
+      <c r="A24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="1:7" s="16" customFormat="1" ht="55.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="10"/>
+      <c r="F26"/>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E27" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-    </row>
-    <row r="33" spans="1:13" ht="4.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="8" t="s">
+    <row r="28" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" ht="4.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="10" t="s">
+    <row r="32" spans="1:7" ht="44.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="F34" s="17" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="F32" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G32" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="17" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="G35" s="18" t="s">
-        <v>6</v>
-      </c>
+    <row r="33" spans="1:13" s="16" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="G33" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="G36" s="11"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="G37" s="11"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="G38" s="11"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="G39" s="11"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="G40" s="11"/>
-    </row>
-    <row r="41" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="G41" s="11"/>
-    </row>
-    <row r="42" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="G42" s="11"/>
-    </row>
-    <row r="43" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:13" ht="2.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" autoFilter="0" selectUnlockedCells="1"/>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A27:G27"/>
   </mergeCells>
-  <conditionalFormatting sqref="A16:E16 G16 A17:G18">
+  <conditionalFormatting sqref="A16:E16 G16">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:O33">
+  <conditionalFormatting sqref="I19:O31">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$I21&lt;&gt;0</formula>
+      <formula>$I19&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N21:N44" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N19:N42" xr:uid="{819A01AB-0010-4633-A6EC-3F42F1A65BB0}">
       <formula1>$I$12</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O21:O44" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
-      <formula1>N21</formula1>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O19:O42" xr:uid="{0D63E666-9414-4358-BF2B-A7FB8B1DA8A8}">
+      <formula1>N19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M21:M43" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M19:M41" xr:uid="{FD5DB15B-7740-4358-85C4-A26F30BA628F}">
       <formula1>"Продавца,Покупателя, -"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L21:L43" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L19:L41" xr:uid="{02A2EAA3-2EA2-4BF3-B5A7-79CAAA73C3F2}">
       <formula1>"Продавца,Покупателя"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K21:K44" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K19:K42" xr:uid="{0083999A-9C9B-4DB7-9798-4B5CB4C21831}">
       <formula1>"с борта,с хранения"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>